<commit_message>
se actualizo transparencia y otros mas
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauragonzalez\Desktop\ESCRITORIO JUNIO 2020\SECRETARÍA EJECUTIVA 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEA6F5A-518D-4CE0-B97B-2F86AB8ED3BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210856CC-BF0F-457E-BF1F-9E28F7713FC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="SECRETARÍA TÉCNICA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'SECRETARÍA TÉCNICA'!$A$2:$Q$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'UNIDAD DE SISTEMAS DE INFORMACI'!$A$2:$Q$18</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -298,13 +298,16 @@
     <t>1.6.10 ACTUALIZACIONES Y MEJORAS</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  Septiembre 2020</t>
-  </si>
-  <si>
     <t>1.2 CORRESPONDENCIA EXTERNA</t>
   </si>
   <si>
     <t>1.2.13 RESPALDO</t>
+  </si>
+  <si>
+    <t>Fecha de Actualización y/o Revisión:  abril 2021</t>
+  </si>
+  <si>
+    <t>Fecha de Actualización y/o Revisión: abril 2021</t>
   </si>
 </sst>
 </file>
@@ -772,6 +775,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,11 +796,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -825,9 +831,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1151,8 +1154,8 @@
   </sheetPr>
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,25 +1180,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1208,25 +1211,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1239,32 +1242,32 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="51" t="s">
         <v>7</v>
       </c>
@@ -1282,37 +1285,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="45" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1327,13 +1330,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1355,9 +1358,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1512,7 +1515,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>26</v>
@@ -30435,12 +30438,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -30452,6 +30449,12 @@
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30466,7 +30469,7 @@
   <dimension ref="A1:AA1048573"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30492,25 +30495,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -30523,25 +30526,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30554,37 +30557,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30597,37 +30600,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30642,13 +30645,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30670,9 +30673,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -31324,7 +31327,7 @@
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
       <c r="D21" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>26</v>
@@ -32434,7 +32437,7 @@
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32460,25 +32463,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -32491,25 +32494,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32522,37 +32525,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32565,37 +32568,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32610,13 +32613,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32638,9 +32641,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34044,7 +34047,7 @@
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34069,25 +34072,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -34100,25 +34103,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34131,37 +34134,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34174,37 +34177,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34219,13 +34222,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34247,9 +34250,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35641,7 +35644,7 @@
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35667,25 +35670,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -35698,25 +35701,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35729,37 +35732,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35772,37 +35775,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35817,13 +35820,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35845,9 +35848,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37356,8 +37359,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37382,25 +37385,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -37413,25 +37416,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37444,37 +37447,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37487,11 +37490,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="63" t="s">
@@ -37500,24 +37503,24 @@
       <c r="G4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37532,11 +37535,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="63"/>
       <c r="G5" s="63"/>
       <c r="H5" s="15" t="s">
@@ -37560,9 +37563,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>

</xml_diff>

<commit_message>
se suben cambis de transparencia
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95DE357-FC85-4620-9972-7646BF00E68D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9D212D9-0C9F-4AAA-8EAD-DF5A6282E011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -304,13 +304,10 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  mayo  2021</t>
+    <t>Fecha de Actualización y/o Revisión:  julio 2021</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: mayo 2021</t>
-  </si>
-  <si>
-    <t>Fecha de Actualización y/o Revisión:  mayo 2021</t>
+    <t>Fecha de Actualización y/o Revisión: julio 2021</t>
   </si>
 </sst>
 </file>
@@ -778,6 +775,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -798,9 +798,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1183,25 +1180,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1214,25 +1211,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1245,37 +1242,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="50" t="s">
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1288,37 +1285,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="44" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1333,13 +1330,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1361,9 +1358,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -30441,6 +30438,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -30457,7 +30455,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30498,25 +30495,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -32409,11 +32406,6 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -32426,6 +32418,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32466,25 +32463,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -34019,11 +34016,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -34036,6 +34028,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34075,25 +34072,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -35616,6 +35613,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
@@ -35632,7 +35630,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35647,7 +35644,7 @@
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35673,25 +35670,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -37332,11 +37329,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -37349,6 +37341,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37388,25 +37385,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -39203,11 +39200,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -39220,6 +39212,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
se suben cambios a transparencia previos a cambios del mes
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9D212D9-0C9F-4AAA-8EAD-DF5A6282E011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19382438-8687-47D3-BD4B-D83C5D1E3C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="SECRETARÍA TÉCNICA" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="86">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -304,10 +304,7 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  julio 2021</t>
-  </si>
-  <si>
-    <t>Fecha de Actualización y/o Revisión: julio 2021</t>
+    <t>Fecha de Actualización y/o Revisión: agosto 2021</t>
   </si>
 </sst>
 </file>
@@ -799,15 +796,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,6 +819,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1154,7 +1151,7 @@
   </sheetPr>
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -30438,6 +30435,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -30454,7 +30452,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30526,25 +30523,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30557,37 +30554,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30600,37 +30597,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="61" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30645,13 +30642,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30673,9 +30670,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32406,6 +32403,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -32422,7 +32420,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32464,7 +32461,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -32494,25 +32491,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32525,37 +32522,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32568,37 +32565,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="61" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32613,13 +32610,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32641,9 +32638,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34016,6 +34013,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -34032,7 +34030,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34103,25 +34100,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34134,37 +34131,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34177,37 +34174,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="61" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34222,13 +34219,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34250,9 +34247,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35613,11 +35610,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -35630,6 +35622,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35671,7 +35668,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -35701,25 +35698,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35732,37 +35729,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35775,37 +35772,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="61" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35820,13 +35817,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35848,9 +35845,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37329,6 +37326,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -37345,7 +37343,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37359,7 +37356,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -37416,25 +37413,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37447,37 +37444,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37490,11 +37487,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="61" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="63" t="s">
@@ -37503,24 +37500,24 @@
       <c r="G4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37535,11 +37532,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="63"/>
       <c r="G5" s="63"/>
       <c r="H5" s="15" t="s">
@@ -37563,9 +37560,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39200,6 +39197,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -39216,7 +39214,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
se baja carpeta 2017
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01B58E29-1BB0-4C4E-ACEC-9D5EB4681FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADF389D-A6D8-4CE1-BD5A-F63CEE46745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="88">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -304,10 +304,13 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  octubre 2021</t>
+    <t>Fecha de Actualización y/o Revisión:  diciembre 2021</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: octubre 2021</t>
+    <t>Fecha de Actualización y/o Revisión: diciembre 2021</t>
+  </si>
+  <si>
+    <t>Fecha de Actualización y/o Revisión:diciembre 2021</t>
   </si>
 </sst>
 </file>
@@ -775,6 +778,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -793,11 +799,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,12 +834,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1155,7 +1158,7 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,25 +1183,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="A1" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1211,25 +1214,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1242,32 +1245,32 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="51" t="s">
         <v>7</v>
       </c>
@@ -1285,37 +1288,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="45" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1330,13 +1333,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1358,9 +1361,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -30438,9 +30441,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -30455,6 +30455,9 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30495,25 +30498,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -30526,25 +30529,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30557,37 +30560,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30600,37 +30603,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30645,13 +30648,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30673,9 +30676,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32406,6 +32409,9 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -32420,9 +32426,6 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32463,25 +32466,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -32494,25 +32497,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32525,37 +32528,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32568,37 +32571,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32613,13 +32616,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32641,9 +32644,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34016,6 +34019,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -34030,9 +34036,6 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34072,25 +34075,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -34103,25 +34106,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34134,37 +34137,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34177,37 +34180,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34222,13 +34225,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34250,9 +34253,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35613,6 +35616,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -35627,9 +35633,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35670,25 +35673,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -35701,25 +35704,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35732,37 +35735,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35775,37 +35778,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35820,13 +35823,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35848,9 +35851,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37329,6 +37332,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -37343,9 +37349,6 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37385,25 +37388,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -37416,25 +37419,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37447,37 +37450,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37490,11 +37493,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="60" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="63" t="s">
@@ -37503,24 +37506,24 @@
       <c r="G4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="53" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37535,11 +37538,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="63"/>
       <c r="G5" s="63"/>
       <c r="H5" s="15" t="s">
@@ -37563,9 +37566,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39200,6 +39203,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -39214,9 +39220,6 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
actualiza trasparencia, se suben 2 boletines y 41 solicitudes de información
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1677F577-FA45-4674-9592-E7199EFB5EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01E97F92-DCD8-4A18-A550-809B611FE356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -304,13 +304,13 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión:MAYO 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión: MAYO 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión:  MAYO 2022</t>
   </si>
 </sst>
 </file>
@@ -773,6 +773,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -788,11 +791,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -823,9 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1175,25 +1175,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1206,25 +1206,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1237,32 +1237,32 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="50" t="s">
         <v>7</v>
       </c>
@@ -1280,37 +1280,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="45" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1325,13 +1325,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1353,9 +1353,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -30433,6 +30433,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
@@ -30449,7 +30450,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30490,25 +30490,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -30521,25 +30521,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30552,37 +30552,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30595,37 +30595,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30640,13 +30640,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30668,9 +30668,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32401,6 +32401,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -32417,7 +32418,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32458,25 +32458,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -32489,25 +32489,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32520,37 +32520,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32563,37 +32563,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32608,13 +32608,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32636,9 +32636,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34011,6 +34011,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -34027,7 +34028,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34067,25 +34067,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -34098,25 +34098,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34129,37 +34129,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34172,37 +34172,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34217,13 +34217,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34245,9 +34245,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35608,6 +35608,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -35624,7 +35625,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35665,25 +35665,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -35696,25 +35696,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35727,37 +35727,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35770,37 +35770,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35815,13 +35815,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35843,9 +35843,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37324,6 +37324,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -37340,7 +37341,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37380,25 +37380,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -37411,25 +37411,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37442,37 +37442,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37485,11 +37485,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="62" t="s">
@@ -37498,24 +37498,24 @@
       <c r="G4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37530,11 +37530,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="62"/>
       <c r="G5" s="62"/>
       <c r="H5" s="15" t="s">
@@ -37558,9 +37558,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39195,6 +39195,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -39211,7 +39212,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se generaron cambios en transparencia septiembre de jurídico
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1CD459-ACDD-4AE4-89BB-81BECDB10A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC8BC21-58A1-4AAE-9D7B-8410BF414728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="SECRETARÍA TÉCNICA" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="88">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -304,16 +304,13 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  agosto 2022</t>
+    <t>Fecha de Actualización y/o Revisión: septiembre 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: agosto 2022</t>
+    <t>Fecha de Actualización y/o Revisión:  septiembre 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: aosto 2022</t>
-  </si>
-  <si>
-    <t>Fecha de Actualización y/o Revisión:agosto 2022</t>
+    <t>Fecha de Actualización y/o Revisión: septiembre  2022</t>
   </si>
 </sst>
 </file>
@@ -649,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -770,11 +767,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -793,9 +790,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,7 +1146,7 @@
   </sheetPr>
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -1179,7 +1173,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1307,13 +1301,13 @@
       </c>
       <c r="M4" s="48"/>
       <c r="N4" s="48"/>
-      <c r="O4" s="50" t="s">
+      <c r="O4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="50" t="s">
+      <c r="P4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="50" t="s">
+      <c r="Q4" s="43" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1356,9 +1350,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1544,9 +1538,9 @@
       <c r="Q10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -30436,6 +30430,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -30452,7 +30447,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30494,7 +30488,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -30524,25 +30518,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30555,37 +30549,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="59" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30598,37 +30592,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30643,13 +30637,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30671,9 +30665,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -31324,7 +31318,7 @@
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="37" t="s">
         <v>84</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -32404,11 +32398,6 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -32421,6 +32410,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32462,7 +32456,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -32492,25 +32486,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32523,37 +32517,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="59" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32566,37 +32560,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32611,13 +32605,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32639,9 +32633,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34014,11 +34008,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -34031,6 +34020,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34071,7 +34065,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -34101,25 +34095,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34132,37 +34126,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="59" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34175,37 +34169,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34220,13 +34214,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34248,9 +34242,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35611,6 +35605,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
@@ -35627,7 +35622,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35669,7 +35663,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -35699,25 +35693,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35730,37 +35724,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="59" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35773,37 +35767,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35818,13 +35812,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35846,9 +35840,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37327,11 +37321,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -37344,6 +37333,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37357,7 +37351,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048574"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -37384,7 +37378,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -37414,25 +37408,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37445,37 +37439,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="59" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37488,37 +37482,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="60" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37533,13 +37527,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -37561,9 +37555,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39198,11 +39192,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -39215,6 +39204,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se suben cambios de administracion a el apartado de transparencia
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC8BC21-58A1-4AAE-9D7B-8410BF414728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E745939E-F469-44A9-98FD-02FCFECAF865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
   <si>
     <t>CATÁLOGO DE DISPOSICIÓN DOCUMENTAL</t>
   </si>
@@ -304,13 +304,10 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: septiembre 2022</t>
+    <t>Fecha de Actualización y/o Revisión: octubre 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  septiembre 2022</t>
-  </si>
-  <si>
-    <t>Fecha de Actualización y/o Revisión: septiembre  2022</t>
+    <t>Fecha de Actualización y/o Revisión:  octubre 2022</t>
   </si>
 </sst>
 </file>
@@ -791,15 +788,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,6 +811,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -30430,6 +30427,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -30446,7 +30444,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30518,25 +30515,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30549,37 +30546,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30592,37 +30589,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30637,13 +30634,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30665,9 +30662,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32398,6 +32395,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -32414,7 +32412,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32486,25 +32483,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32517,37 +32514,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32560,37 +32557,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32605,13 +32602,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32633,9 +32630,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34008,6 +34005,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -34024,7 +34022,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34095,25 +34092,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34126,37 +34123,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34169,37 +34166,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34214,13 +34211,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34242,9 +34239,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35605,11 +35602,6 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -35622,6 +35614,11 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35663,7 +35660,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -35693,25 +35690,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35724,37 +35721,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35767,37 +35764,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35812,13 +35809,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35840,9 +35837,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37321,6 +37318,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -37337,7 +37335,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37378,7 +37375,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -37408,25 +37405,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37439,37 +37436,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37482,11 +37479,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="56" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="61" t="s">
@@ -37495,24 +37492,24 @@
       <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51" t="s">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37527,11 +37524,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="61"/>
       <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
@@ -37555,9 +37552,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39192,6 +39189,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -39208,7 +39206,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>